<commit_message>
retrieve all from Stage2
</commit_message>
<xml_diff>
--- a/force-app/main/default/staticresources/Physical_Activity_Challenge_Tracker.xlsx
+++ b/force-app/main/default/staticresources/Physical_Activity_Challenge_Tracker.xlsx
@@ -1,23 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\1929 - NCAI TRAIL Program 2020-2021\Training and Technical Assistance\Help Documents\Final Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brand\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFFD5F2-B4D2-4F11-8619-09E3EA213664}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{14A46852-F86B-4DC3-8FED-056910C1487B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="2355" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
-    <sheet name="Physical Activity Challenges" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="4" state="hidden" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="Strenth Challenges" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -78,7 +85,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -110,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -125,7 +132,35 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -137,7 +172,7 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -147,12 +182,25 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -162,13 +210,114 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -188,161 +337,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -358,103 +352,83 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <mruColors>
-      <color rgb="FF65B767"/>
-    </mruColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -786,37 +760,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" customWidth="1"/>
     <col min="15" max="15" width="12" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12" customWidth="1"/>
     <col min="19" max="19" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>16</v>
       </c>
@@ -839,7 +813,7 @@
       <c r="R1" s="12"/>
       <c r="S1" s="12"/>
     </row>
-    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
@@ -886,7 +860,7 @@
       </c>
       <c r="S2" s="18"/>
     </row>
-    <row r="3" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="22"/>
       <c r="B3" s="14" t="s">
         <v>13</v>
@@ -943,7 +917,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="6"/>
@@ -964,7 +938,7 @@
       <c r="R4" s="6"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="8"/>
@@ -985,7 +959,7 @@
       <c r="R5" s="8"/>
       <c r="S5" s="9"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="8"/>
@@ -1006,7 +980,7 @@
       <c r="R6" s="8"/>
       <c r="S6" s="9"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="8"/>
@@ -1027,7 +1001,7 @@
       <c r="R7" s="8"/>
       <c r="S7" s="9"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="8"/>
@@ -1048,7 +1022,7 @@
       <c r="R8" s="8"/>
       <c r="S8" s="9"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="8"/>
@@ -1069,7 +1043,7 @@
       <c r="R9" s="8"/>
       <c r="S9" s="9"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="8"/>
@@ -1090,7 +1064,7 @@
       <c r="R10" s="8"/>
       <c r="S10" s="9"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="8"/>
@@ -1111,7 +1085,7 @@
       <c r="R11" s="8"/>
       <c r="S11" s="9"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="8"/>
@@ -1132,7 +1106,7 @@
       <c r="R12" s="8"/>
       <c r="S12" s="9"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="8"/>
@@ -1153,7 +1127,7 @@
       <c r="R13" s="8"/>
       <c r="S13" s="9"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="8"/>
@@ -1174,7 +1148,7 @@
       <c r="R14" s="8"/>
       <c r="S14" s="9"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="8"/>
@@ -1195,7 +1169,7 @@
       <c r="R15" s="8"/>
       <c r="S15" s="9"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="8"/>
@@ -1216,7 +1190,7 @@
       <c r="R16" s="8"/>
       <c r="S16" s="9"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="8"/>
@@ -1237,7 +1211,7 @@
       <c r="R17" s="8"/>
       <c r="S17" s="9"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="8"/>
@@ -1258,7 +1232,7 @@
       <c r="R18" s="8"/>
       <c r="S18" s="9"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="8"/>
@@ -1279,7 +1253,7 @@
       <c r="R19" s="8"/>
       <c r="S19" s="9"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="8"/>
@@ -1300,7 +1274,7 @@
       <c r="R20" s="8"/>
       <c r="S20" s="9"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="8"/>
@@ -1321,7 +1295,7 @@
       <c r="R21" s="8"/>
       <c r="S21" s="9"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="8"/>
@@ -1342,7 +1316,7 @@
       <c r="R22" s="8"/>
       <c r="S22" s="9"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="8"/>
@@ -1363,7 +1337,7 @@
       <c r="R23" s="8"/>
       <c r="S23" s="9"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="8"/>
@@ -1384,7 +1358,7 @@
       <c r="R24" s="8"/>
       <c r="S24" s="9"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="8"/>
@@ -1405,8 +1379,8 @@
       <c r="R25" s="8"/>
       <c r="S25" s="9"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
+    <row r="26" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="3"/>
       <c r="B26" s="2"/>
       <c r="C26" s="8"/>
       <c r="D26" s="9"/>
@@ -1426,8 +1400,7 @@
       <c r="R26" s="8"/>
       <c r="S26" s="9"/>
     </row>
-    <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="24"/>
+    <row r="27" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="3"/>
       <c r="C27" s="10"/>
       <c r="D27" s="11"/>
@@ -1447,7 +1420,7 @@
       <c r="R27" s="10"/>
       <c r="S27" s="11"/>
     </row>
-    <row r="29" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
@@ -1467,7 +1440,7 @@
       <c r="R29"/>
       <c r="S29"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -1507,26 +1480,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{065B55A2-E6A7-4306-8ED6-9DBEE7E724C4}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>